<commit_message>
edit togel pecah 2d
</commit_message>
<xml_diff>
--- a/dataset/togel7.xlsx
+++ b/dataset/togel7.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1161"/>
+  <dimension ref="A1:G1162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41916,6 +41916,43 @@
         </is>
       </c>
     </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1162" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="E1162" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F1162" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="G1162" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>